<commit_message>
exclude NA form proportions in report 2, update results report 3 (one more response included)
</commit_message>
<xml_diff>
--- a/data/clean/Delphi3_counts.xlsx
+++ b/data/clean/Delphi3_counts.xlsx
@@ -1834,7 +1834,7 @@
         <v>447</v>
       </c>
       <c r="F2" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="3">
@@ -1854,7 +1854,7 @@
         <v>447</v>
       </c>
       <c r="F3" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="4">
@@ -1874,7 +1874,7 @@
         <v>447</v>
       </c>
       <c r="F4" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="5">
@@ -1894,7 +1894,7 @@
         <v>447</v>
       </c>
       <c r="F5" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="6">
@@ -1934,7 +1934,7 @@
         <v>578</v>
       </c>
       <c r="F7" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="8">
@@ -2014,7 +2014,7 @@
         <v>578</v>
       </c>
       <c r="F11" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="12">
@@ -2054,7 +2054,7 @@
         <v>578</v>
       </c>
       <c r="F13" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="14">
@@ -2134,7 +2134,7 @@
         <v>447</v>
       </c>
       <c r="F17" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="18">
@@ -2194,7 +2194,7 @@
         <v>578</v>
       </c>
       <c r="F20" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="21">
@@ -2234,7 +2234,7 @@
         <v>578</v>
       </c>
       <c r="F22" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="23">
@@ -2254,7 +2254,7 @@
         <v>447</v>
       </c>
       <c r="F23" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="24">
@@ -2294,7 +2294,7 @@
         <v>447</v>
       </c>
       <c r="F25" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="26">
@@ -2334,7 +2334,7 @@
         <v>578</v>
       </c>
       <c r="F27" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="28">
@@ -2354,7 +2354,7 @@
         <v>447</v>
       </c>
       <c r="F28" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="29">
@@ -2414,7 +2414,7 @@
         <v>578</v>
       </c>
       <c r="F31" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="32">
@@ -2494,7 +2494,7 @@
         <v>447</v>
       </c>
       <c r="F35" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="36">
@@ -2514,7 +2514,7 @@
         <v>447</v>
       </c>
       <c r="F36" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="37">
@@ -2574,7 +2574,7 @@
         <v>578</v>
       </c>
       <c r="F39" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="40">
@@ -2634,7 +2634,7 @@
         <v>447</v>
       </c>
       <c r="F42" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="43">
@@ -2694,7 +2694,7 @@
         <v>447</v>
       </c>
       <c r="F45" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="46">
@@ -2754,7 +2754,7 @@
         <v>447</v>
       </c>
       <c r="F48" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="49">
@@ -2914,7 +2914,7 @@
         <v>578</v>
       </c>
       <c r="F56" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="57">
@@ -3034,7 +3034,7 @@
         <v>578</v>
       </c>
       <c r="F62" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="63">
@@ -3094,7 +3094,7 @@
         <v>578</v>
       </c>
       <c r="F65" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="66">
@@ -3194,7 +3194,7 @@
         <v>459</v>
       </c>
       <c r="F70" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="71">
@@ -3214,7 +3214,7 @@
         <v>578</v>
       </c>
       <c r="F71" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="72">
@@ -3254,7 +3254,7 @@
         <v>447</v>
       </c>
       <c r="F73" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="74">
@@ -3274,7 +3274,7 @@
         <v>447</v>
       </c>
       <c r="F74" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="75">
@@ -3374,7 +3374,7 @@
         <v>578</v>
       </c>
       <c r="F79" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="80">
@@ -3394,7 +3394,7 @@
         <v>447</v>
       </c>
       <c r="F80" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="81">
@@ -3434,7 +3434,7 @@
         <v>447</v>
       </c>
       <c r="F82" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="83">
@@ -3514,7 +3514,7 @@
         <v>447</v>
       </c>
       <c r="F86" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="87">
@@ -3594,7 +3594,7 @@
         <v>447</v>
       </c>
       <c r="F90" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="91">
@@ -3674,7 +3674,7 @@
         <v>447</v>
       </c>
       <c r="F94" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="95">
@@ -3734,7 +3734,7 @@
         <v>447</v>
       </c>
       <c r="F97" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="98">
@@ -3774,7 +3774,7 @@
         <v>578</v>
       </c>
       <c r="F99" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="100">
@@ -3814,7 +3814,7 @@
         <v>578</v>
       </c>
       <c r="F101" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="102">
@@ -3894,7 +3894,7 @@
         <v>578</v>
       </c>
       <c r="F105" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="106">
@@ -3934,7 +3934,7 @@
         <v>447</v>
       </c>
       <c r="F107" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="108">
@@ -3974,7 +3974,7 @@
         <v>578</v>
       </c>
       <c r="F109" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="110">
@@ -4014,7 +4014,7 @@
         <v>578</v>
       </c>
       <c r="F111" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="112">
@@ -4054,7 +4054,7 @@
         <v>578</v>
       </c>
       <c r="F113" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="114">
@@ -4094,7 +4094,7 @@
         <v>578</v>
       </c>
       <c r="F115" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="116">
@@ -4134,7 +4134,7 @@
         <v>447</v>
       </c>
       <c r="F117" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="118">
@@ -4214,7 +4214,7 @@
         <v>578</v>
       </c>
       <c r="F121" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="122">
@@ -4234,7 +4234,7 @@
         <v>447</v>
       </c>
       <c r="F122" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="123">
@@ -4274,7 +4274,7 @@
         <v>447</v>
       </c>
       <c r="F124" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="125">
@@ -4294,7 +4294,7 @@
         <v>447</v>
       </c>
       <c r="F125" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="126">
@@ -4334,7 +4334,7 @@
         <v>578</v>
       </c>
       <c r="F127" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="128">
@@ -4374,7 +4374,7 @@
         <v>578</v>
       </c>
       <c r="F129" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="130">
@@ -4414,7 +4414,7 @@
         <v>578</v>
       </c>
       <c r="F131" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="132">
@@ -4494,7 +4494,7 @@
         <v>578</v>
       </c>
       <c r="F135" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="136">
@@ -4554,7 +4554,7 @@
         <v>578</v>
       </c>
       <c r="F138" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="139">
@@ -4594,7 +4594,7 @@
         <v>447</v>
       </c>
       <c r="F140" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="141">
@@ -4654,7 +4654,7 @@
         <v>578</v>
       </c>
       <c r="F143" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="144">
@@ -4714,7 +4714,7 @@
         <v>578</v>
       </c>
       <c r="F146" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="147">
@@ -4754,7 +4754,7 @@
         <v>578</v>
       </c>
       <c r="F148" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="149">
@@ -4854,7 +4854,7 @@
         <v>578</v>
       </c>
       <c r="F153" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="154">
@@ -4954,7 +4954,7 @@
         <v>578</v>
       </c>
       <c r="F158" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="159">
@@ -5014,7 +5014,7 @@
         <v>578</v>
       </c>
       <c r="F161" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="162">
@@ -5054,7 +5054,7 @@
         <v>578</v>
       </c>
       <c r="F163" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="164">
@@ -5074,7 +5074,7 @@
         <v>447</v>
       </c>
       <c r="F164" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="165">
@@ -5174,7 +5174,7 @@
         <v>578</v>
       </c>
       <c r="F169" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="170">
@@ -5254,7 +5254,7 @@
         <v>578</v>
       </c>
       <c r="F173" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="174">
@@ -5354,7 +5354,7 @@
         <v>578</v>
       </c>
       <c r="F178" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="179">
@@ -5374,7 +5374,7 @@
         <v>447</v>
       </c>
       <c r="F179" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="180">
@@ -5394,7 +5394,7 @@
         <v>447</v>
       </c>
       <c r="F180" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="181">
@@ -5474,7 +5474,7 @@
         <v>578</v>
       </c>
       <c r="F184" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="185">
@@ -5574,7 +5574,7 @@
         <v>578</v>
       </c>
       <c r="F189" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="190">
@@ -5654,7 +5654,7 @@
         <v>578</v>
       </c>
       <c r="F193" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="194">
@@ -5734,7 +5734,7 @@
         <v>578</v>
       </c>
       <c r="F197" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="198">
@@ -5814,7 +5814,7 @@
         <v>578</v>
       </c>
       <c r="F201" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="202">
@@ -5854,7 +5854,7 @@
         <v>578</v>
       </c>
       <c r="F203" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="204">
@@ -5894,7 +5894,7 @@
         <v>578</v>
       </c>
       <c r="F205" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="206">
@@ -5974,7 +5974,7 @@
         <v>578</v>
       </c>
       <c r="F209" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="210">
@@ -6034,7 +6034,7 @@
         <v>578</v>
       </c>
       <c r="F212" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="213">
@@ -6134,7 +6134,7 @@
         <v>578</v>
       </c>
       <c r="F217" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="218">
@@ -6214,7 +6214,7 @@
         <v>578</v>
       </c>
       <c r="F221" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="222">
@@ -6274,7 +6274,7 @@
         <v>578</v>
       </c>
       <c r="F224" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="225">
@@ -6314,7 +6314,7 @@
         <v>447</v>
       </c>
       <c r="F226" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="227">
@@ -6334,7 +6334,7 @@
         <v>447</v>
       </c>
       <c r="F227" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="228">
@@ -6374,7 +6374,7 @@
         <v>578</v>
       </c>
       <c r="F229" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="230">
@@ -6414,7 +6414,7 @@
         <v>578</v>
       </c>
       <c r="F231" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="232">
@@ -6434,7 +6434,7 @@
         <v>447</v>
       </c>
       <c r="F232" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="233">
@@ -6454,7 +6454,7 @@
         <v>447</v>
       </c>
       <c r="F233" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="234">
@@ -6494,7 +6494,7 @@
         <v>578</v>
       </c>
       <c r="F235" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="236">
@@ -6534,7 +6534,7 @@
         <v>578</v>
       </c>
       <c r="F237" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="238">
@@ -6614,7 +6614,7 @@
         <v>578</v>
       </c>
       <c r="F241" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="242">
@@ -6654,7 +6654,7 @@
         <v>447</v>
       </c>
       <c r="F243" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="244">
@@ -6694,7 +6694,7 @@
         <v>578</v>
       </c>
       <c r="F245" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="246">
@@ -6714,7 +6714,7 @@
         <v>447</v>
       </c>
       <c r="F246" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="247">
@@ -6754,7 +6754,7 @@
         <v>578</v>
       </c>
       <c r="F248" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="249">
@@ -6794,7 +6794,7 @@
         <v>578</v>
       </c>
       <c r="F250" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="251">
@@ -6874,7 +6874,7 @@
         <v>578</v>
       </c>
       <c r="F254" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="255">

</xml_diff>